<commit_message>
fix(JdT): mise à jour du journal de travail
</commit_message>
<xml_diff>
--- a/P_Bulles-Flashcard/T-P_Bulles-Flashcards-MatiasDenis-JDT.xlsx
+++ b/P_Bulles-Flashcard/T-P_Bulles-Flashcards-MatiasDenis-JDT.xlsx
@@ -5,10 +5,10 @@
   <workbookPr updateLinks="never" codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pb58unc\Desktop\P_Bulles-Flashcards\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pb58unc\Desktop\P_Bulles-Flashcards\P_Bulles-Flashcard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90CF78DD-F452-4661-82A6-236BED1ECB39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC8EAB09-AA4C-40DB-8D17-B1720B1916A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-225" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="47">
   <si>
     <t>Module :</t>
   </si>
@@ -201,6 +201,12 @@
   </si>
   <si>
     <t>Création d'un repo github afin de pouvoir voir les avancées du projet.</t>
+  </si>
+  <si>
+    <t>Avancées dans les steps 4 à 11</t>
+  </si>
+  <si>
+    <t>à compléter</t>
   </si>
 </sst>
 </file>
@@ -1779,7 +1785,7 @@
   <dimension ref="A1:G54"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" topLeftCell="A9" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -2113,7 +2119,9 @@
       <c r="B28" s="79">
         <v>8</v>
       </c>
-      <c r="C28" s="71"/>
+      <c r="C28" s="71" t="s">
+        <v>45</v>
+      </c>
       <c r="D28" s="59"/>
       <c r="E28" s="59"/>
       <c r="F28" s="59"/>
@@ -2405,27 +2413,27 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="15365" r:id="rId5" name="btnCreateWorkSheet">
+        <control shapeId="15364" r:id="rId5" name="btnCreatePlanning">
           <controlPr defaultSize="0" autoLine="0" r:id="rId6">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>8</xdr:row>
-                <xdr:rowOff>190500</xdr:rowOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>6</xdr:col>
-                <xdr:colOff>114300</xdr:colOff>
-                <xdr:row>10</xdr:row>
-                <xdr:rowOff>152400</xdr:rowOff>
+                <xdr:colOff>95250</xdr:colOff>
+                <xdr:row>7</xdr:row>
+                <xdr:rowOff>47625</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="15365" r:id="rId5" name="btnCreateWorkSheet"/>
+        <control shapeId="15364" r:id="rId5" name="btnCreatePlanning"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -2455,27 +2463,27 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="15364" r:id="rId9" name="btnCreatePlanning">
+        <control shapeId="15365" r:id="rId9" name="btnCreateWorkSheet">
           <controlPr defaultSize="0" autoLine="0" r:id="rId10">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
+                <xdr:row>8</xdr:row>
+                <xdr:rowOff>190500</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>6</xdr:col>
-                <xdr:colOff>95250</xdr:colOff>
-                <xdr:row>7</xdr:row>
-                <xdr:rowOff>47625</xdr:rowOff>
+                <xdr:colOff>114300</xdr:colOff>
+                <xdr:row>10</xdr:row>
+                <xdr:rowOff>152400</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="15364" r:id="rId9" name="btnCreatePlanning"/>
+        <control shapeId="15365" r:id="rId9" name="btnCreateWorkSheet"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -3185,7 +3193,7 @@
   <dimension ref="A1:H153"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -3592,10 +3600,16 @@
       </c>
       <c r="D41" s="9"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="1"/>
-      <c r="B42" s="2"/>
-      <c r="C42" s="10"/>
+    <row r="42" spans="1:8" ht="27" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B42" s="2">
+        <v>11</v>
+      </c>
+      <c r="C42" s="95" t="s">
+        <v>46</v>
+      </c>
       <c r="D42" s="10"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
@@ -3682,7 +3696,7 @@
       </c>
       <c r="B56" s="47">
         <f>SUM(B41:B55)</f>
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="C56" s="87" t="s">
         <v>31</v>
@@ -4671,6 +4685,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="bf2f2df3-a963-4452-b0e7-67dabc627c35">
@@ -4679,15 +4702,6 @@
     <TaxCatchAll xmlns="f7d9f5a6-831d-4621-8c77-cbcaf993e406" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4710,6 +4724,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{483719EA-391A-4C4B-985B-9805B7FCB9D5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C29126A-0525-4FCA-A870-5924A033DD5A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -4718,12 +4740,4 @@
     <ds:schemaRef ds:uri="f7d9f5a6-831d-4621-8c77-cbcaf993e406"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{483719EA-391A-4C4B-985B-9805B7FCB9D5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
doc(JdT et cahier des charges): mise à jour du journal de travail et relecture du cahier des charges
</commit_message>
<xml_diff>
--- a/P_Bulles-Flashcard/T-P_Bulles-Flashcards-MatiasDenis-JDT.xlsx
+++ b/P_Bulles-Flashcard/T-P_Bulles-Flashcards-MatiasDenis-JDT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pb58unc\Desktop\P_Bulles-Flashcards\P_Bulles-Flashcard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC8EAB09-AA4C-40DB-8D17-B1720B1916A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D5BEA19-AAB7-4E65-B275-17A036861D0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-225" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="51">
   <si>
     <t>Module :</t>
   </si>
@@ -173,12 +173,6 @@
     <t>Lecture et prise de connaissance de tous les aspects demandés pour ce projet.</t>
   </si>
   <si>
-    <t>Création de l'infrastructure de base</t>
-  </si>
-  <si>
-    <t>Création de l'infrastructure de base sur l'application du projet grâce aux steps 0 et 1.</t>
-  </si>
-  <si>
     <t>Création d'un layout, composant layout et partials</t>
   </si>
   <si>
@@ -206,7 +200,25 @@
     <t>Avancées dans les steps 4 à 11</t>
   </si>
   <si>
-    <t>à compléter</t>
+    <t>Création de l'infrastructure de base sur l'application test grâce aux steps 0 et 1.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sans trop entrer dans le détail, ont été suivis les steps depuis la fin du 4 jusqu'à la fin du 11. Ce qui a été créé, entre autres: step5: création d'un jeu de données avec seeder et factory, step6: afficher les détails des enseignants avec route, méthodes dans le contrôleur, ajout d'une vue, step 7: suppression d'un enseignant, création d'une route, ajout d'une méthode au contrôleur, step8: ajout d'un enseignant, création de deux routes (une pour afficher le formulaire pour les informations de l'enseignant, une pour gérer l'ajout de l'enseignant), ajout d'un validateur, des méthodes au contrôleur, ajout d'une vue, step 9:  ajout d'un enseignant, création de deux routes (une pour afficher le formulaire pour les informations de l'enseignant, une pour gérer l'ajout de l'enseignant), ajout d'un validateur, des méthodes au contrôleur, step 10: mise en place de l'authentification, mise à jour de la table t_user, création de migration user, seeder, step 11: mise en place du login, nouvelle route, </t>
+  </si>
+  <si>
+    <t>nouveau contrôleur et méthode, création d'un validateur, step 12: mise en place du logout, nouvelle route, nouvelle méthode AuthControlleur, step 13: gestion des rôles, utilisation des middlewares (un pour partager l'état de l'authentification, un pour vérifier le rôle)</t>
+  </si>
+  <si>
+    <t>Finalisation des step 11 à 13</t>
+  </si>
+  <si>
+    <t>Création de l'infrastructure de l'application test</t>
+  </si>
+  <si>
+    <t>création d'un nouveau contrôleur et méthode, création d'un validateur pour finaliser le step 11, step 12: mise en place du logout, nouvelle route, nouvelle méthode AuthControlleur, step 13: gestion des rôles, utilisation des middlewares (un pour partager l'état de l'authentification, un pour vérifier le rôle)</t>
+  </si>
+  <si>
+    <t>Création de l'infrastructure du projet Flashcards</t>
   </si>
 </sst>
 </file>
@@ -1784,8 +1796,8 @@
   </sheetPr>
   <dimension ref="A1:G54"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A9" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A11" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -2055,7 +2067,7 @@
         <v>3</v>
       </c>
       <c r="C23" s="70" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="D23" s="59"/>
       <c r="E23" s="59"/>
@@ -2068,7 +2080,7 @@
         <v>4</v>
       </c>
       <c r="C24" s="70" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D24" s="59"/>
       <c r="E24" s="59"/>
@@ -2081,7 +2093,7 @@
         <v>5</v>
       </c>
       <c r="C25" s="70" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D25" s="59"/>
       <c r="E25" s="59"/>
@@ -2094,7 +2106,7 @@
         <v>6</v>
       </c>
       <c r="C26" s="70" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D26" s="59"/>
       <c r="E26" s="59"/>
@@ -2107,7 +2119,7 @@
         <v>7</v>
       </c>
       <c r="C27" s="70" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D27" s="59"/>
       <c r="E27" s="59"/>
@@ -2120,7 +2132,7 @@
         <v>8</v>
       </c>
       <c r="C28" s="71" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D28" s="59"/>
       <c r="E28" s="59"/>
@@ -2132,7 +2144,9 @@
       <c r="B29" s="81">
         <v>9</v>
       </c>
-      <c r="C29" s="71"/>
+      <c r="C29" s="71" t="s">
+        <v>47</v>
+      </c>
       <c r="D29" s="59"/>
       <c r="E29" s="59"/>
       <c r="F29" s="59"/>
@@ -2143,7 +2157,9 @@
       <c r="B30" s="79">
         <v>10</v>
       </c>
-      <c r="C30" s="70"/>
+      <c r="C30" s="70" t="s">
+        <v>50</v>
+      </c>
       <c r="D30" s="59"/>
       <c r="E30" s="59"/>
       <c r="F30" s="59"/>
@@ -2413,27 +2429,27 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="15364" r:id="rId5" name="btnCreatePlanning">
+        <control shapeId="15365" r:id="rId5" name="btnCreateWorkSheet">
           <controlPr defaultSize="0" autoLine="0" r:id="rId6">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
+                <xdr:row>8</xdr:row>
+                <xdr:rowOff>190500</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>6</xdr:col>
-                <xdr:colOff>95250</xdr:colOff>
-                <xdr:row>7</xdr:row>
-                <xdr:rowOff>47625</xdr:rowOff>
+                <xdr:colOff>114300</xdr:colOff>
+                <xdr:row>10</xdr:row>
+                <xdr:rowOff>152400</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="15364" r:id="rId5" name="btnCreatePlanning"/>
+        <control shapeId="15365" r:id="rId5" name="btnCreateWorkSheet"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -2463,27 +2479,27 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="15365" r:id="rId9" name="btnCreateWorkSheet">
+        <control shapeId="15364" r:id="rId9" name="btnCreatePlanning">
           <controlPr defaultSize="0" autoLine="0" r:id="rId10">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>8</xdr:row>
-                <xdr:rowOff>190500</xdr:rowOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>6</xdr:col>
-                <xdr:colOff>114300</xdr:colOff>
-                <xdr:row>10</xdr:row>
-                <xdr:rowOff>152400</xdr:rowOff>
+                <xdr:colOff>95250</xdr:colOff>
+                <xdr:row>7</xdr:row>
+                <xdr:rowOff>47625</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="15365" r:id="rId9" name="btnCreateWorkSheet"/>
+        <control shapeId="15364" r:id="rId9" name="btnCreatePlanning"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -3192,8 +3208,8 @@
   <sheetPr codeName="Feuil9"/>
   <dimension ref="A1:H153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="A61" sqref="A61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -3404,25 +3420,25 @@
     </row>
     <row r="24" spans="1:8" ht="40.5" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="B24" s="2">
         <v>3</v>
       </c>
       <c r="C24" s="95" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="D24" s="10"/>
     </row>
     <row r="25" spans="1:8" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B25" s="2">
         <v>3</v>
       </c>
       <c r="C25" s="95" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D25" s="10"/>
       <c r="F25" s="31"/>
@@ -3431,13 +3447,13 @@
     </row>
     <row r="26" spans="1:8" ht="40.5" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B26" s="2">
         <v>1</v>
       </c>
       <c r="C26" s="95" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D26" s="10"/>
       <c r="F26" s="34"/>
@@ -3446,13 +3462,13 @@
     </row>
     <row r="27" spans="1:8" ht="40.5" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B27" s="2">
         <v>2</v>
       </c>
       <c r="C27" s="95" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D27" s="10"/>
       <c r="F27" s="36"/>
@@ -3590,25 +3606,25 @@
     </row>
     <row r="41" spans="1:8" ht="27" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B41" s="4">
         <v>1</v>
       </c>
       <c r="C41" s="88" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D41" s="9"/>
     </row>
-    <row r="42" spans="1:8" ht="27" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" ht="162" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B42" s="2">
         <v>11</v>
       </c>
       <c r="C42" s="95" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D42" s="10"/>
     </row>
@@ -3738,14 +3754,22 @@
         <v>13</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="5"/>
-      <c r="B60" s="4"/>
-      <c r="C60" s="88"/>
+    <row r="60" spans="1:4" ht="54" x14ac:dyDescent="0.25">
+      <c r="A60" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B60" s="4">
+        <v>6</v>
+      </c>
+      <c r="C60" s="88" t="s">
+        <v>49</v>
+      </c>
       <c r="D60" s="90"/>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="1"/>
+    <row r="61" spans="1:4" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>50</v>
+      </c>
       <c r="B61" s="2"/>
       <c r="C61" s="10"/>
       <c r="D61" s="10"/>
@@ -3834,7 +3858,7 @@
       </c>
       <c r="B75" s="47">
         <f>SUM(B60:B74)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C75" s="87" t="s">
         <v>31</v>
@@ -3879,7 +3903,9 @@
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="5"/>
       <c r="B79" s="4"/>
-      <c r="C79" s="88"/>
+      <c r="C79" s="88" t="s">
+        <v>46</v>
+      </c>
       <c r="D79" s="9"/>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
@@ -4685,15 +4711,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="bf2f2df3-a963-4452-b0e7-67dabc627c35">
@@ -4702,6 +4719,15 @@
     <TaxCatchAll xmlns="f7d9f5a6-831d-4621-8c77-cbcaf993e406" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4724,14 +4750,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{483719EA-391A-4C4B-985B-9805B7FCB9D5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C29126A-0525-4FCA-A870-5924A033DD5A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -4740,4 +4758,12 @@
     <ds:schemaRef ds:uri="f7d9f5a6-831d-4621-8c77-cbcaf993e406"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{483719EA-391A-4C4B-985B-9805B7FCB9D5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>